<commit_message>
Original bert with 14 layers added. 1GB hard limit
</commit_message>
<xml_diff>
--- a/image_preprocessing/two_vertex/accuracy_degradation/physical/bert24.xlsx
+++ b/image_preprocessing/two_vertex/accuracy_degradation/physical/bert24.xlsx
@@ -530,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,10 +615,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>11.70829057693481</v>
+        <v>14.76951837539673</v>
       </c>
       <c r="G4" t="n">
-        <v>222.1422130391735</v>
+        <v>253.0900819532456</v>
       </c>
     </row>
     <row r="5">
@@ -644,10 +644,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>14.25635576248169</v>
+        <v>13.0419921875</v>
       </c>
       <c r="G5" t="n">
-        <v>286.845679865946</v>
+        <v>335.6222380587877</v>
       </c>
     </row>
     <row r="6">
@@ -673,10 +673,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>15.24913311004638</v>
+        <v>16.8469214439392</v>
       </c>
       <c r="G6" t="n">
-        <v>395.92399640919</v>
+        <v>406.1006340094022</v>
       </c>
     </row>
     <row r="7">
@@ -702,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>21.36382818222045</v>
+        <v>25.46954631805419</v>
       </c>
       <c r="G7" t="n">
-        <v>471.1062309111347</v>
+        <v>453.0762011590305</v>
       </c>
     </row>
     <row r="8">
@@ -719,7 +719,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sentimental-bert24-2/bert24_p2_stage0</t>
+          <t>Sentimental-bert24-2/bert</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -731,10 +731,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>34.10517692565918</v>
+        <v>29.32890415191649</v>
       </c>
       <c r="G8" t="n">
-        <v>63.4736076074188</v>
+        <v>54.79022872335062</v>
       </c>
     </row>
     <row r="9">
@@ -748,7 +748,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sentimental-bert24-2/bert24_p2_stage0</t>
+          <t>Sentimental-bert24-2/bert</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -760,10 +760,10 @@
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>37.86195993423461</v>
+        <v>35.04937648773193</v>
       </c>
       <c r="G9" t="n">
-        <v>102.0931224308183</v>
+        <v>98.68201533690643</v>
       </c>
     </row>
     <row r="10">
@@ -777,7 +777,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sentimental-bert24-2/bert24_p2_stage0</t>
+          <t>Sentimental-bert24-2/bert</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -789,10 +789,10 @@
         <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>44.0561819076538</v>
+        <v>30.60036420822144</v>
       </c>
       <c r="G10" t="n">
-        <v>155.2255058841154</v>
+        <v>171.6389662108538</v>
       </c>
     </row>
     <row r="11">
@@ -806,7 +806,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sentimental-bert24-2/bert24_p2_stage0</t>
+          <t>Sentimental-bert24-2/bert</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -818,126 +818,10 @@
         <v>8</v>
       </c>
       <c r="F11" t="n">
-        <v>56.66375160217285</v>
+        <v>46.12188577651977</v>
       </c>
       <c r="G11" t="n">
-        <v>204.3747050205778</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2/bert24-p2-stage1</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Tesla P40</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="n">
-        <v>19.61172103881835</v>
-      </c>
-      <c r="G12" t="n">
-        <v>124.3240481007306</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2/bert24-p2-stage1</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Tesla P40</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>2</v>
-      </c>
-      <c r="F13" t="n">
-        <v>21.42068862915039</v>
-      </c>
-      <c r="G13" t="n">
-        <v>204.8301444362955</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2/bert24-p2-stage1</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Tesla P40</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>4</v>
-      </c>
-      <c r="F14" t="n">
-        <v>26.99255228042602</v>
-      </c>
-      <c r="G14" t="n">
-        <v>272.9883957750656</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Sentimental-bert24-2/bert24-p2-stage1</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Tesla P40</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>8</v>
-      </c>
-      <c r="F15" t="n">
-        <v>39.54147338867185</v>
-      </c>
-      <c r="G15" t="n">
-        <v>332.7173933219876</v>
+        <v>216.6269201778877</v>
       </c>
     </row>
   </sheetData>
@@ -1010,7 +894,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{"Sentimental-bert24-2/tokenizer": {"CPU1": {"THROUGHPUT": [[1, 222.14221303917353], [2, 286.84567986594595], [4, 395.92399640918995], [8, 471.10623091113473]], "LATENCY": [[1, 11.708290576934806], [2, 14.256355762481686], [4, 15.249133110046385], [8, 21.363828182220452]]}}, "Sentimental-bert24-2/bert24_p2_stage0": {"Tesla P40": {"THROUGHPUT": [[1, 63.4736076074188], [2, 102.0931224308183], [4, 155.22550588411542], [8, 204.37470502057778]], "LATENCY": [[1, 34.10517692565918], [2, 37.86195993423461], [4, 44.0561819076538], [8, 56.66375160217285]]}}, "Sentimental-bert24-2/bert24-p2-stage1": {"Tesla P40": {"THROUGHPUT": [[1, 124.32404810073064], [2, 204.83014443629546], [4, 272.98839577506556], [8, 332.7173933219876]], "LATENCY": [[1, 19.611721038818352], [2, 21.42068862915039], [4, 26.992552280426022], [8, 39.541473388671854]]}}}</t>
+          <t>{"Sentimental-bert24-2/tokenizer": {"CPU1": {"THROUGHPUT": [[1, 253.09008195324557], [2, 335.62223805878773], [4, 406.1006340094022], [8, 453.0762011590305]], "LATENCY": [[1, 14.769518375396727], [2, 13.041992187499998], [4, 16.846921443939202], [8, 25.469546318054185]]}}, "Sentimental-bert24-2/bert": {"Tesla P40": {"THROUGHPUT": [[1, 54.790228723350616], [2, 98.68201533690643], [4, 171.6389662108538], [8, 216.6269201778877]], "LATENCY": [[1, 29.328904151916493], [2, 35.04937648773193], [4, 30.600364208221436], [8, 46.12188577651977]]}}}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
p99 p95 are way off
</commit_message>
<xml_diff>
--- a/image_preprocessing/two_vertex/accuracy_degradation/physical/bert24.xlsx
+++ b/image_preprocessing/two_vertex/accuracy_degradation/physical/bert24.xlsx
@@ -615,10 +615,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>11.70829057693481</v>
+        <v>15.76137065887451</v>
       </c>
       <c r="G4" t="n">
-        <v>222.1422130391735</v>
+        <v>230.6125734453858</v>
       </c>
     </row>
     <row r="5">
@@ -644,10 +644,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>14.25635576248169</v>
+        <v>21.6904091835022</v>
       </c>
       <c r="G5" t="n">
-        <v>286.845679865946</v>
+        <v>273.1469391460485</v>
       </c>
     </row>
     <row r="6">
@@ -673,10 +673,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>15.24913311004638</v>
+        <v>24.83202219009399</v>
       </c>
       <c r="G6" t="n">
-        <v>395.92399640919</v>
+        <v>381.4970774020932</v>
       </c>
     </row>
     <row r="7">
@@ -702,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>21.36382818222045</v>
+        <v>26.2183928489685</v>
       </c>
       <c r="G7" t="n">
-        <v>471.1062309111347</v>
+        <v>429.5303772916355</v>
       </c>
     </row>
     <row r="8">
@@ -731,10 +731,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>34.10517692565918</v>
+        <v>25.70167064666748</v>
       </c>
       <c r="G8" t="n">
-        <v>63.4736076074188</v>
+        <v>90.43009740517203</v>
       </c>
     </row>
     <row r="9">
@@ -760,10 +760,10 @@
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>37.86195993423461</v>
+        <v>29.12822961807251</v>
       </c>
       <c r="G9" t="n">
-        <v>102.0931224308183</v>
+        <v>137.2221240733107</v>
       </c>
     </row>
     <row r="10">
@@ -789,10 +789,10 @@
         <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>44.0561819076538</v>
+        <v>34.91165161132812</v>
       </c>
       <c r="G10" t="n">
-        <v>155.2255058841154</v>
+        <v>182.5665340188121</v>
       </c>
     </row>
     <row r="11">
@@ -818,10 +818,10 @@
         <v>8</v>
       </c>
       <c r="F11" t="n">
-        <v>56.66375160217285</v>
+        <v>52.65275239944457</v>
       </c>
       <c r="G11" t="n">
-        <v>204.3747050205778</v>
+        <v>246.5175600174442</v>
       </c>
     </row>
     <row r="12">
@@ -847,10 +847,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>19.61172103881835</v>
+        <v>22.60903596878051</v>
       </c>
       <c r="G12" t="n">
-        <v>124.3240481007306</v>
+        <v>102.7385153817363</v>
       </c>
     </row>
     <row r="13">
@@ -876,10 +876,10 @@
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>21.42068862915039</v>
+        <v>25.35673141479492</v>
       </c>
       <c r="G13" t="n">
-        <v>204.8301444362955</v>
+        <v>179.7882116347376</v>
       </c>
     </row>
     <row r="14">
@@ -905,10 +905,10 @@
         <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>26.99255228042602</v>
+        <v>29.36871290206909</v>
       </c>
       <c r="G14" t="n">
-        <v>272.9883957750656</v>
+        <v>259.6441140147517</v>
       </c>
     </row>
     <row r="15">
@@ -934,10 +934,10 @@
         <v>8</v>
       </c>
       <c r="F15" t="n">
-        <v>39.54147338867185</v>
+        <v>39.58753108978271</v>
       </c>
       <c r="G15" t="n">
-        <v>332.7173933219876</v>
+        <v>342.2610144325105</v>
       </c>
     </row>
   </sheetData>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{"Sentimental-bert24-2/tokenizer": {"CPU1": {"THROUGHPUT": [[1, 222.14221303917353], [2, 286.84567986594595], [4, 395.92399640918995], [8, 471.10623091113473]], "LATENCY": [[1, 11.708290576934806], [2, 14.256355762481686], [4, 15.249133110046385], [8, 21.363828182220452]]}}, "Sentimental-bert24-2/bert24_p2_stage0": {"Tesla P40": {"THROUGHPUT": [[1, 63.4736076074188], [2, 102.0931224308183], [4, 155.22550588411542], [8, 204.37470502057778]], "LATENCY": [[1, 34.10517692565918], [2, 37.86195993423461], [4, 44.0561819076538], [8, 56.66375160217285]]}}, "Sentimental-bert24-2/bert24-p2-stage1": {"Tesla P40": {"THROUGHPUT": [[1, 124.32404810073064], [2, 204.83014443629546], [4, 272.98839577506556], [8, 332.7173933219876]], "LATENCY": [[1, 19.611721038818352], [2, 21.42068862915039], [4, 26.992552280426022], [8, 39.541473388671854]]}}}</t>
+          <t>{"Sentimental-bert24-2/tokenizer": {"CPU1": {"THROUGHPUT": [[1, 230.61257344538583], [2, 273.1469391460485], [4, 381.49707740209317], [8, 429.53037729163555]], "LATENCY": [[1, 15.761370658874512], [2, 21.690409183502197], [4, 24.832022190093994], [8, 26.218392848968495]]}}, "Sentimental-bert24-2/bert24_p2_stage0": {"Tesla P40": {"THROUGHPUT": [[1, 90.43009740517203], [2, 137.22212407331068], [4, 182.56653401881212], [8, 246.51756001744423]], "LATENCY": [[1, 25.70167064666748], [2, 29.128229618072506], [4, 34.91165161132812], [8, 52.652752399444566]]}}, "Sentimental-bert24-2/bert24-p2-stage1": {"Tesla P40": {"THROUGHPUT": [[1, 102.7385153817363], [2, 179.78821163473765], [4, 259.6441140147517], [8, 342.26101443251054]], "LATENCY": [[1, 22.609035968780514], [2, 25.356731414794922], [4, 29.36871290206909], [8, 39.587531089782715]]}}}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>